<commit_message>
Data Structures 2016 final content + exam problems.
</commit_message>
<xml_diff>
--- a/4. Data Structures/DS Efficiency.xlsx
+++ b/4. Data Structures/DS Efficiency.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gad\Dropbox\SoftUni\4. Data Structures\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\SoftUni\4. Data Structures\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="59">
   <si>
     <t>Array</t>
   </si>
@@ -195,13 +195,19 @@
   </si>
   <si>
     <t>Elements ordered by key + dictionary goodies + fast subrange.</t>
+  </si>
+  <si>
+    <t>*SortedDictionary does not support Range operation.</t>
+  </si>
+  <si>
+    <t>*SortedSet is faster than OrderedSet</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -216,6 +222,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -251,7 +264,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -271,6 +284,7 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -551,10 +565,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H17"/>
+  <dimension ref="A1:H20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G26" sqref="G26"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -968,8 +982,18 @@
         <v>50</v>
       </c>
     </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" s="9" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" s="9" t="s">
+        <v>58</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>